<commit_message>
Fixed editing Diknas courses
</commit_message>
<xml_diff>
--- a/lib/tasks/DiknasConversions.xlsx
+++ b/lib/tasks/DiknasConversions.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="77">
   <si>
     <t>AGAMA</t>
   </si>
@@ -322,566 +319,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="A2">
-            <v>25</v>
-          </cell>
-          <cell r="B2" t="str">
-            <v>AGAMA</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D2">
-            <v>1</v>
-          </cell>
-          <cell r="E2">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>26</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>BAHASA INDONESIA</v>
-          </cell>
-          <cell r="C3" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D3">
-            <v>1</v>
-          </cell>
-          <cell r="E3">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>27</v>
-          </cell>
-          <cell r="B4" t="str">
-            <v>BAHASA INGGRIS</v>
-          </cell>
-          <cell r="C4" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D4">
-            <v>1</v>
-          </cell>
-          <cell r="E4">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>28</v>
-          </cell>
-          <cell r="B5" t="str">
-            <v>BIOLOGI</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D5">
-            <v>1</v>
-          </cell>
-          <cell r="E5">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>29</v>
-          </cell>
-          <cell r="B6" t="str">
-            <v>EKONOMI</v>
-          </cell>
-          <cell r="C6" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D6">
-            <v>1</v>
-          </cell>
-          <cell r="E6">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>30</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>FISIKA</v>
-          </cell>
-          <cell r="C7" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D7">
-            <v>1</v>
-          </cell>
-          <cell r="E7">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>31</v>
-          </cell>
-          <cell r="B8" t="str">
-            <v>GEOGRAFI</v>
-          </cell>
-          <cell r="C8" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D8">
-            <v>1</v>
-          </cell>
-          <cell r="E8">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>32</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>KIMIA</v>
-          </cell>
-          <cell r="C9" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D9">
-            <v>1</v>
-          </cell>
-          <cell r="E9">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10">
-            <v>33</v>
-          </cell>
-          <cell r="B10" t="str">
-            <v>MATEMATIKA</v>
-          </cell>
-          <cell r="C10" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D10">
-            <v>1</v>
-          </cell>
-          <cell r="E10">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="A11">
-            <v>34</v>
-          </cell>
-          <cell r="B11" t="str">
-            <v xml:space="preserve">PENDIDIKAN JASMANI </v>
-          </cell>
-          <cell r="C11" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D11">
-            <v>1</v>
-          </cell>
-          <cell r="E11">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="A12">
-            <v>35</v>
-          </cell>
-          <cell r="B12" t="str">
-            <v>PENDIDIKAN KEWARGANEGARAAN</v>
-          </cell>
-          <cell r="C12" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D12">
-            <v>1</v>
-          </cell>
-          <cell r="E12">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="A13">
-            <v>36</v>
-          </cell>
-          <cell r="B13" t="str">
-            <v>SEJARAH</v>
-          </cell>
-          <cell r="C13" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D13">
-            <v>1</v>
-          </cell>
-          <cell r="E13">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="A14">
-            <v>37</v>
-          </cell>
-          <cell r="B14" t="str">
-            <v>SENI BUDAYA</v>
-          </cell>
-          <cell r="C14" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D14">
-            <v>1</v>
-          </cell>
-          <cell r="E14">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="A15">
-            <v>38</v>
-          </cell>
-          <cell r="B15" t="str">
-            <v>SOSIOLOGI</v>
-          </cell>
-          <cell r="C15" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D15">
-            <v>1</v>
-          </cell>
-          <cell r="E15">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="A16">
-            <v>39</v>
-          </cell>
-          <cell r="B16" t="str">
-            <v>TEKNOLOGI INFORMASI</v>
-          </cell>
-          <cell r="C16" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D16">
-            <v>1</v>
-          </cell>
-          <cell r="E16">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="A17">
-            <v>40</v>
-          </cell>
-          <cell r="B17" t="str">
-            <v>KETERAMPILAN</v>
-          </cell>
-          <cell r="C17" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D17">
-            <v>1</v>
-          </cell>
-          <cell r="E17">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="A18">
-            <v>41</v>
-          </cell>
-          <cell r="B18" t="str">
-            <v>AGAMA</v>
-          </cell>
-          <cell r="C18" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D18">
-            <v>2</v>
-          </cell>
-          <cell r="E18">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="A19">
-            <v>42</v>
-          </cell>
-          <cell r="B19" t="str">
-            <v>BAHASA INDONESIA</v>
-          </cell>
-          <cell r="C19" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D19">
-            <v>2</v>
-          </cell>
-          <cell r="E19">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="A20">
-            <v>43</v>
-          </cell>
-          <cell r="B20" t="str">
-            <v>BAHASA INGGRIS</v>
-          </cell>
-          <cell r="C20" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D20">
-            <v>2</v>
-          </cell>
-          <cell r="E20">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="21">
-          <cell r="A21">
-            <v>44</v>
-          </cell>
-          <cell r="B21" t="str">
-            <v>BIOLOGI</v>
-          </cell>
-          <cell r="C21" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D21">
-            <v>2</v>
-          </cell>
-          <cell r="E21">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="A22">
-            <v>45</v>
-          </cell>
-          <cell r="B22" t="str">
-            <v>EKONOMI</v>
-          </cell>
-          <cell r="C22" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D22">
-            <v>2</v>
-          </cell>
-          <cell r="E22">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="A23">
-            <v>46</v>
-          </cell>
-          <cell r="B23" t="str">
-            <v>FISIKA</v>
-          </cell>
-          <cell r="C23" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D23">
-            <v>2</v>
-          </cell>
-          <cell r="E23">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="A24">
-            <v>47</v>
-          </cell>
-          <cell r="B24" t="str">
-            <v>GEOGRAFI</v>
-          </cell>
-          <cell r="C24" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D24">
-            <v>2</v>
-          </cell>
-          <cell r="E24">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="A25">
-            <v>48</v>
-          </cell>
-          <cell r="B25" t="str">
-            <v>KIMIA</v>
-          </cell>
-          <cell r="C25" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D25">
-            <v>2</v>
-          </cell>
-          <cell r="E25">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="26">
-          <cell r="A26">
-            <v>49</v>
-          </cell>
-          <cell r="B26" t="str">
-            <v>MATEMATIKA</v>
-          </cell>
-          <cell r="C26" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D26">
-            <v>2</v>
-          </cell>
-          <cell r="E26">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="A27">
-            <v>50</v>
-          </cell>
-          <cell r="B27" t="str">
-            <v xml:space="preserve">PENDIDIKAN JASMANI </v>
-          </cell>
-          <cell r="C27" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D27">
-            <v>2</v>
-          </cell>
-          <cell r="E27">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="A28">
-            <v>51</v>
-          </cell>
-          <cell r="B28" t="str">
-            <v>PENDIDIKAN KEWARGANEGARAAN</v>
-          </cell>
-          <cell r="C28" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D28">
-            <v>2</v>
-          </cell>
-          <cell r="E28">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="A29">
-            <v>52</v>
-          </cell>
-          <cell r="B29" t="str">
-            <v>SEJARAH</v>
-          </cell>
-          <cell r="C29" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D29">
-            <v>2</v>
-          </cell>
-          <cell r="E29">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="A30">
-            <v>53</v>
-          </cell>
-          <cell r="B30" t="str">
-            <v>SENI BUDAYA</v>
-          </cell>
-          <cell r="C30" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D30">
-            <v>2</v>
-          </cell>
-          <cell r="E30">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="A31">
-            <v>54</v>
-          </cell>
-          <cell r="B31" t="str">
-            <v>SOSIOLOGI</v>
-          </cell>
-          <cell r="C31" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D31">
-            <v>2</v>
-          </cell>
-          <cell r="E31">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="32">
-          <cell r="A32">
-            <v>55</v>
-          </cell>
-          <cell r="B32" t="str">
-            <v>TEKNOLOGI INFORMASI</v>
-          </cell>
-          <cell r="C32" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D32">
-            <v>2</v>
-          </cell>
-          <cell r="E32">
-            <v>12</v>
-          </cell>
-        </row>
-        <row r="33">
-          <cell r="A33">
-            <v>56</v>
-          </cell>
-          <cell r="B33" t="str">
-            <v>KETERAMPILAN</v>
-          </cell>
-          <cell r="C33" t="str">
-            <v>2017-2018</v>
-          </cell>
-          <cell r="D33">
-            <v>2</v>
-          </cell>
-          <cell r="E33">
-            <v>12</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1149,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46:I87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1200,9 +637,6 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="1">
-        <v>25</v>
-      </c>
       <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
@@ -1215,23 +649,17 @@
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <f>VLOOKUP($A2,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I2" s="1">
-        <f>VLOOKUP($A2,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
       <c r="J2" s="1">
-        <f>VLOOKUP($A2,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="1">
-        <v>35</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1244,23 +672,17 @@
       <c r="G3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f>VLOOKUP($A3,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I3" s="1">
-        <f>VLOOKUP($A3,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
       <c r="J3" s="1">
-        <f>VLOOKUP($A3,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="1">
-        <v>35</v>
-      </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
@@ -1273,23 +695,17 @@
       <c r="G4" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="1" t="str">
-        <f>VLOOKUP($A4,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I4" s="1">
-        <f>VLOOKUP($A4,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" s="1">
-        <f>VLOOKUP($A4,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="1">
-        <v>26</v>
-      </c>
       <c r="B5" s="1" t="s">
         <v>44</v>
       </c>
@@ -1302,23 +718,17 @@
       <c r="G5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="1" t="str">
-        <f>VLOOKUP($A5,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I5" s="1">
-        <f>VLOOKUP($A5,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" s="1">
-        <f>VLOOKUP($A5,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="1">
-        <v>27</v>
-      </c>
       <c r="B6" s="1" t="s">
         <v>45</v>
       </c>
@@ -1331,23 +741,17 @@
       <c r="G6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="1" t="str">
-        <f>VLOOKUP($A6,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I6" s="1">
-        <f>VLOOKUP($A6,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" s="1">
-        <f>VLOOKUP($A6,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="1">
-        <v>33</v>
-      </c>
       <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
@@ -1360,23 +764,17 @@
       <c r="G7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="1" t="str">
-        <f>VLOOKUP($A7,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I7" s="1">
-        <f>VLOOKUP($A7,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" s="1">
-        <f>VLOOKUP($A7,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="1">
-        <v>33</v>
-      </c>
       <c r="B8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1389,23 +787,17 @@
       <c r="G8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="1" t="str">
-        <f>VLOOKUP($A8,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I8" s="1">
-        <f>VLOOKUP($A8,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" s="1">
-        <f>VLOOKUP($A8,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="1">
-        <v>33</v>
-      </c>
       <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
@@ -1418,23 +810,17 @@
       <c r="G9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="1" t="str">
-        <f>VLOOKUP($A9,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I9" s="1">
-        <f>VLOOKUP($A9,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
       <c r="J9" s="1">
-        <f>VLOOKUP($A9,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="1">
-        <v>33</v>
-      </c>
       <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
@@ -1447,23 +833,17 @@
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H10" s="1" t="str">
-        <f>VLOOKUP($A10,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I10" s="1">
-        <f>VLOOKUP($A10,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10">
         <v>1</v>
       </c>
       <c r="J10" s="1">
-        <f>VLOOKUP($A10,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="1">
-        <v>30</v>
-      </c>
       <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
@@ -1476,23 +856,17 @@
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="1" t="str">
-        <f>VLOOKUP($A11,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I11" s="1">
-        <f>VLOOKUP($A11,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11">
         <v>1</v>
       </c>
       <c r="J11" s="1">
-        <f>VLOOKUP($A11,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="1">
-        <v>32</v>
-      </c>
       <c r="B12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1505,23 +879,17 @@
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="1" t="str">
-        <f>VLOOKUP($A12,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I12" s="1">
-        <f>VLOOKUP($A12,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12">
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <f>VLOOKUP($A12,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="1">
-        <v>28</v>
-      </c>
       <c r="B13" s="1" t="s">
         <v>51</v>
       </c>
@@ -1534,23 +902,17 @@
       <c r="G13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H13" s="1" t="str">
-        <f>VLOOKUP($A13,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I13" s="1">
-        <f>VLOOKUP($A13,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13">
         <v>1</v>
       </c>
       <c r="J13" s="1">
-        <f>VLOOKUP($A13,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="1">
-        <v>31</v>
-      </c>
       <c r="B14" s="1" t="s">
         <v>52</v>
       </c>
@@ -1563,23 +925,17 @@
       <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H14" s="1" t="str">
-        <f>VLOOKUP($A14,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I14" s="1">
-        <f>VLOOKUP($A14,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14">
         <v>1</v>
       </c>
       <c r="J14" s="1">
-        <f>VLOOKUP($A14,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="1">
-        <v>29</v>
-      </c>
       <c r="B15" s="1" t="s">
         <v>53</v>
       </c>
@@ -1592,23 +948,17 @@
       <c r="G15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="1" t="str">
-        <f>VLOOKUP($A15,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I15" s="1">
-        <f>VLOOKUP($A15,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15">
         <v>1</v>
       </c>
       <c r="J15" s="1">
-        <f>VLOOKUP($A15,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="1">
-        <v>29</v>
-      </c>
       <c r="B16" s="1" t="s">
         <v>54</v>
       </c>
@@ -1621,23 +971,17 @@
       <c r="G16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H16" s="1" t="str">
-        <f>VLOOKUP($A16,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I16" s="1">
-        <f>VLOOKUP($A16,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16">
         <v>1</v>
       </c>
       <c r="J16" s="1">
-        <f>VLOOKUP($A16,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="1">
-        <v>38</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
       <c r="B17" s="1" t="s">
         <v>55</v>
       </c>
@@ -1650,23 +994,17 @@
       <c r="G17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H17" s="1" t="str">
-        <f>VLOOKUP($A17,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I17" s="1">
-        <f>VLOOKUP($A17,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17">
         <v>1</v>
       </c>
       <c r="J17" s="1">
-        <f>VLOOKUP($A17,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="1">
-        <v>36</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
@@ -1679,23 +1017,17 @@
       <c r="G18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="1" t="str">
-        <f>VLOOKUP($A18,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I18" s="1">
-        <f>VLOOKUP($A18,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18">
         <v>1</v>
       </c>
       <c r="J18" s="1">
-        <f>VLOOKUP($A18,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="1">
-        <v>39</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
       <c r="B19" s="1" t="s">
         <v>57</v>
       </c>
@@ -1708,23 +1040,17 @@
       <c r="G19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H19" s="1" t="str">
-        <f>VLOOKUP($A19,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I19" s="1">
-        <f>VLOOKUP($A19,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19">
         <v>1</v>
       </c>
       <c r="J19" s="1">
-        <f>VLOOKUP($A19,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1737,23 +1063,17 @@
       <c r="G20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="1" t="str">
-        <f>VLOOKUP($A20,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I20" s="1">
-        <f>VLOOKUP($A20,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20">
         <v>1</v>
       </c>
       <c r="J20" s="1">
-        <f>VLOOKUP($A20,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
       <c r="B21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1766,23 +1086,17 @@
       <c r="G21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="1" t="str">
-        <f>VLOOKUP($A21,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I21" s="1">
-        <f>VLOOKUP($A21,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H21" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21">
         <v>1</v>
       </c>
       <c r="J21" s="1">
-        <f>VLOOKUP($A21,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
       <c r="B22" s="1" t="s">
         <v>58</v>
       </c>
@@ -1795,23 +1109,17 @@
       <c r="G22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H22" s="1" t="str">
-        <f>VLOOKUP($A22,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I22" s="1">
-        <f>VLOOKUP($A22,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22">
         <v>1</v>
       </c>
       <c r="J22" s="1">
-        <f>VLOOKUP($A22,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
       <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
@@ -1824,23 +1132,17 @@
       <c r="G23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="1" t="str">
-        <f>VLOOKUP($A23,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I23" s="1">
-        <f>VLOOKUP($A23,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H23" t="s">
+        <v>38</v>
+      </c>
+      <c r="I23">
         <v>1</v>
       </c>
       <c r="J23" s="1">
-        <f>VLOOKUP($A23,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
       <c r="B24" s="1" t="s">
         <v>16</v>
       </c>
@@ -1853,23 +1155,17 @@
       <c r="G24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="1" t="str">
-        <f>VLOOKUP($A24,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I24" s="1">
-        <f>VLOOKUP($A24,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H24" t="s">
+        <v>38</v>
+      </c>
+      <c r="I24">
         <v>1</v>
       </c>
       <c r="J24" s="1">
-        <f>VLOOKUP($A24,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
       <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
@@ -1882,23 +1178,17 @@
       <c r="G25" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="1" t="str">
-        <f>VLOOKUP($A25,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I25" s="1">
-        <f>VLOOKUP($A25,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H25" t="s">
+        <v>38</v>
+      </c>
+      <c r="I25">
         <v>1</v>
       </c>
       <c r="J25" s="1">
-        <f>VLOOKUP($A25,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1911,23 +1201,17 @@
       <c r="G26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H26" s="1" t="str">
-        <f>VLOOKUP($A26,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I26" s="1">
-        <f>VLOOKUP($A26,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26">
         <v>1</v>
       </c>
       <c r="J26" s="1">
-        <f>VLOOKUP($A26,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
       <c r="B27" s="1" t="s">
         <v>13</v>
       </c>
@@ -1940,23 +1224,17 @@
       <c r="G27" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="1" t="str">
-        <f>VLOOKUP($A27,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I27" s="1">
-        <f>VLOOKUP($A27,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H27" t="s">
+        <v>38</v>
+      </c>
+      <c r="I27">
         <v>1</v>
       </c>
       <c r="J27" s="1">
-        <f>VLOOKUP($A27,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
       <c r="B28" s="1" t="s">
         <v>58</v>
       </c>
@@ -1969,23 +1247,17 @@
       <c r="G28" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="1" t="str">
-        <f>VLOOKUP($A28,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I28" s="1">
-        <f>VLOOKUP($A28,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H28" t="s">
+        <v>38</v>
+      </c>
+      <c r="I28">
         <v>1</v>
       </c>
       <c r="J28" s="1">
-        <f>VLOOKUP($A28,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
       <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
@@ -1998,23 +1270,17 @@
       <c r="G29" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="1" t="str">
-        <f>VLOOKUP($A29,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I29" s="1">
-        <f>VLOOKUP($A29,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H29" t="s">
+        <v>38</v>
+      </c>
+      <c r="I29">
         <v>1</v>
       </c>
       <c r="J29" s="1">
-        <f>VLOOKUP($A29,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
       <c r="B30" s="1" t="s">
         <v>16</v>
       </c>
@@ -2027,23 +1293,17 @@
       <c r="G30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="1" t="str">
-        <f>VLOOKUP($A30,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I30" s="1">
-        <f>VLOOKUP($A30,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H30" t="s">
+        <v>38</v>
+      </c>
+      <c r="I30">
         <v>1</v>
       </c>
       <c r="J30" s="1">
-        <f>VLOOKUP($A30,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="1">
-        <v>37</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
       <c r="B31" s="1" t="s">
         <v>60</v>
       </c>
@@ -2056,23 +1316,17 @@
       <c r="G31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="1" t="str">
-        <f>VLOOKUP($A31,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I31" s="1">
-        <f>VLOOKUP($A31,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H31" t="s">
+        <v>38</v>
+      </c>
+      <c r="I31">
         <v>1</v>
       </c>
       <c r="J31" s="1">
-        <f>VLOOKUP($A31,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="1">
-        <v>34</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
       <c r="B32" s="1" t="s">
         <v>18</v>
       </c>
@@ -2085,23 +1339,17 @@
       <c r="G32" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H32" s="1" t="str">
-        <f>VLOOKUP($A32,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I32" s="1">
-        <f>VLOOKUP($A32,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H32" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32">
         <v>1</v>
       </c>
       <c r="J32" s="1">
-        <f>VLOOKUP($A32,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="A33" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10">
       <c r="B33" s="1" t="s">
         <v>12</v>
       </c>
@@ -2114,23 +1362,17 @@
       <c r="G33" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="1" t="str">
-        <f>VLOOKUP($A33,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I33" s="1">
-        <f>VLOOKUP($A33,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33">
         <v>1</v>
       </c>
       <c r="J33" s="1">
-        <f>VLOOKUP($A33,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="A34" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10">
       <c r="B34" s="1" t="s">
         <v>13</v>
       </c>
@@ -2143,23 +1385,17 @@
       <c r="G34" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H34" s="1" t="str">
-        <f>VLOOKUP($A34,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I34" s="1">
-        <f>VLOOKUP($A34,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H34" t="s">
+        <v>38</v>
+      </c>
+      <c r="I34">
         <v>1</v>
       </c>
       <c r="J34" s="1">
-        <f>VLOOKUP($A34,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="A35" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10">
       <c r="B35" s="1" t="s">
         <v>58</v>
       </c>
@@ -2172,23 +1408,17 @@
       <c r="G35" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H35" s="1" t="str">
-        <f>VLOOKUP($A35,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I35" s="1">
-        <f>VLOOKUP($A35,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H35" t="s">
+        <v>38</v>
+      </c>
+      <c r="I35">
         <v>1</v>
       </c>
       <c r="J35" s="1">
-        <f>VLOOKUP($A35,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
-      <c r="A36" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10">
       <c r="B36" s="1" t="s">
         <v>59</v>
       </c>
@@ -2201,23 +1431,17 @@
       <c r="G36" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="1" t="str">
-        <f>VLOOKUP($A36,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I36" s="1">
-        <f>VLOOKUP($A36,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H36" t="s">
+        <v>38</v>
+      </c>
+      <c r="I36">
         <v>1</v>
       </c>
       <c r="J36" s="1">
-        <f>VLOOKUP($A36,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
-      <c r="A37" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
         <v>16</v>
       </c>
@@ -2230,23 +1454,17 @@
       <c r="G37" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="1" t="str">
-        <f>VLOOKUP($A37,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I37" s="1">
-        <f>VLOOKUP($A37,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H37" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37">
         <v>1</v>
       </c>
       <c r="J37" s="1">
-        <f>VLOOKUP($A37,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="A38" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10">
       <c r="B38" s="1" t="s">
         <v>60</v>
       </c>
@@ -2259,23 +1477,17 @@
       <c r="G38" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="1" t="str">
-        <f>VLOOKUP($A38,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I38" s="1">
-        <f>VLOOKUP($A38,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H38" t="s">
+        <v>38</v>
+      </c>
+      <c r="I38">
         <v>1</v>
       </c>
       <c r="J38" s="1">
-        <f>VLOOKUP($A38,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
-      <c r="A39" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10">
       <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
@@ -2288,23 +1500,17 @@
       <c r="G39" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="1" t="str">
-        <f>VLOOKUP($A39,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I39" s="1">
-        <f>VLOOKUP($A39,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39">
         <v>1</v>
       </c>
       <c r="J39" s="1">
-        <f>VLOOKUP($A39,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10">
       <c r="B40" s="1" t="s">
         <v>13</v>
       </c>
@@ -2317,23 +1523,17 @@
       <c r="G40" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="1" t="str">
-        <f>VLOOKUP($A40,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I40" s="1">
-        <f>VLOOKUP($A40,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40">
         <v>1</v>
       </c>
       <c r="J40" s="1">
-        <f>VLOOKUP($A40,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10">
       <c r="B41" s="1" t="s">
         <v>58</v>
       </c>
@@ -2346,23 +1546,17 @@
       <c r="G41" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H41" s="1" t="str">
-        <f>VLOOKUP($A41,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I41" s="1">
-        <f>VLOOKUP($A41,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H41" t="s">
+        <v>38</v>
+      </c>
+      <c r="I41">
         <v>1</v>
       </c>
       <c r="J41" s="1">
-        <f>VLOOKUP($A41,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10">
       <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
@@ -2375,23 +1569,17 @@
       <c r="G42" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H42" s="1" t="str">
-        <f>VLOOKUP($A42,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I42" s="1">
-        <f>VLOOKUP($A42,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I42">
         <v>1</v>
       </c>
       <c r="J42" s="1">
-        <f>VLOOKUP($A42,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10">
       <c r="B43" s="1" t="s">
         <v>16</v>
       </c>
@@ -2404,23 +1592,17 @@
       <c r="G43" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H43" s="1" t="str">
-        <f>VLOOKUP($A43,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I43" s="1">
-        <f>VLOOKUP($A43,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H43" t="s">
+        <v>38</v>
+      </c>
+      <c r="I43">
         <v>1</v>
       </c>
       <c r="J43" s="1">
-        <f>VLOOKUP($A43,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="1">
-        <v>40</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10">
       <c r="B44" s="1" t="s">
         <v>60</v>
       </c>
@@ -2433,23 +1615,17 @@
       <c r="G44" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H44" s="1" t="str">
-        <f>VLOOKUP($A44,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
-      </c>
-      <c r="I44" s="1">
-        <f>VLOOKUP($A44,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
+      <c r="H44" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44">
         <v>1</v>
       </c>
       <c r="J44" s="1">
-        <f>VLOOKUP($A44,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
-      <c r="A45" s="1">
-        <v>41</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10">
       <c r="B45" s="1" t="s">
         <v>40</v>
       </c>
@@ -2462,23 +1638,17 @@
       <c r="G45" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H45" s="1" t="str">
-        <f>VLOOKUP($A45,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H45" t="s">
+        <v>38</v>
       </c>
       <c r="I45" s="1">
-        <f>VLOOKUP($A45,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J45" s="1">
-        <f>VLOOKUP($A45,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="1">
-        <v>51</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10">
       <c r="B46" s="1" t="s">
         <v>41</v>
       </c>
@@ -2491,23 +1661,17 @@
       <c r="G46" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H46" s="1" t="str">
-        <f>VLOOKUP($A46,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H46" t="s">
+        <v>38</v>
       </c>
       <c r="I46" s="1">
-        <f>VLOOKUP($A46,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J46" s="1">
-        <f>VLOOKUP($A46,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="1">
-        <v>51</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10">
       <c r="B47" s="1" t="s">
         <v>20</v>
       </c>
@@ -2520,23 +1684,17 @@
       <c r="G47" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H47" s="1" t="str">
-        <f>VLOOKUP($A47,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H47" t="s">
+        <v>38</v>
       </c>
       <c r="I47" s="1">
-        <f>VLOOKUP($A47,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J47" s="1">
-        <f>VLOOKUP($A47,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="1">
-        <v>42</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10">
       <c r="B48" s="1" t="s">
         <v>44</v>
       </c>
@@ -2549,23 +1707,17 @@
       <c r="G48" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H48" s="1" t="str">
-        <f>VLOOKUP($A48,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H48" t="s">
+        <v>38</v>
       </c>
       <c r="I48" s="1">
-        <f>VLOOKUP($A48,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J48" s="1">
-        <f>VLOOKUP($A48,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="1">
-        <v>43</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10">
       <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
@@ -2578,23 +1730,17 @@
       <c r="G49" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H49" s="1" t="str">
-        <f>VLOOKUP($A49,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H49" t="s">
+        <v>38</v>
       </c>
       <c r="I49" s="1">
-        <f>VLOOKUP($A49,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J49" s="1">
-        <f>VLOOKUP($A49,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="1">
-        <v>49</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10">
       <c r="B50" s="1" t="s">
         <v>46</v>
       </c>
@@ -2607,23 +1753,17 @@
       <c r="G50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H50" s="1" t="str">
-        <f>VLOOKUP($A50,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H50" t="s">
+        <v>38</v>
       </c>
       <c r="I50" s="1">
-        <f>VLOOKUP($A50,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J50" s="1">
-        <f>VLOOKUP($A50,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10">
       <c r="B51" s="1" t="s">
         <v>47</v>
       </c>
@@ -2636,23 +1776,17 @@
       <c r="G51" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H51" s="1" t="str">
-        <f>VLOOKUP($A51,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H51" t="s">
+        <v>38</v>
       </c>
       <c r="I51" s="1">
-        <f>VLOOKUP($A51,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J51" s="1">
-        <f>VLOOKUP($A51,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
-      <c r="A52" s="1">
-        <v>49</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10">
       <c r="B52" s="1" t="s">
         <v>48</v>
       </c>
@@ -2665,23 +1799,17 @@
       <c r="G52" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H52" s="1" t="str">
-        <f>VLOOKUP($A52,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H52" t="s">
+        <v>38</v>
       </c>
       <c r="I52" s="1">
-        <f>VLOOKUP($A52,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J52" s="1">
-        <f>VLOOKUP($A52,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="1">
-        <v>49</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" spans="2:10">
       <c r="B53" s="1" t="s">
         <v>47</v>
       </c>
@@ -2694,23 +1822,17 @@
       <c r="G53" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H53" s="1" t="str">
-        <f>VLOOKUP($A53,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H53" t="s">
+        <v>38</v>
       </c>
       <c r="I53" s="1">
-        <f>VLOOKUP($A53,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J53" s="1">
-        <f>VLOOKUP($A53,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
-      <c r="A54" s="1">
-        <v>46</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="54" spans="2:10">
       <c r="B54" s="1" t="s">
         <v>49</v>
       </c>
@@ -2723,23 +1845,17 @@
       <c r="G54" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H54" s="1" t="str">
-        <f>VLOOKUP($A54,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H54" t="s">
+        <v>38</v>
       </c>
       <c r="I54" s="1">
-        <f>VLOOKUP($A54,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J54" s="1">
-        <f>VLOOKUP($A54,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
-      <c r="A55" s="1">
-        <v>48</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="2:10">
       <c r="B55" s="1" t="s">
         <v>50</v>
       </c>
@@ -2752,23 +1868,17 @@
       <c r="G55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H55" s="1" t="str">
-        <f>VLOOKUP($A55,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H55" t="s">
+        <v>38</v>
       </c>
       <c r="I55" s="1">
-        <f>VLOOKUP($A55,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J55" s="1">
-        <f>VLOOKUP($A55,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="1">
-        <v>44</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10">
       <c r="B56" s="1" t="s">
         <v>51</v>
       </c>
@@ -2781,23 +1891,17 @@
       <c r="G56" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H56" s="1" t="str">
-        <f>VLOOKUP($A56,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H56" t="s">
+        <v>38</v>
       </c>
       <c r="I56" s="1">
-        <f>VLOOKUP($A56,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J56" s="1">
-        <f>VLOOKUP($A56,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
-      <c r="A57" s="1">
-        <v>47</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="2:10">
       <c r="B57" s="1" t="s">
         <v>52</v>
       </c>
@@ -2810,23 +1914,17 @@
       <c r="G57" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H57" s="1" t="str">
-        <f>VLOOKUP($A57,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H57" t="s">
+        <v>38</v>
       </c>
       <c r="I57" s="1">
-        <f>VLOOKUP($A57,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J57" s="1">
-        <f>VLOOKUP($A57,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
-      <c r="A58" s="1">
-        <v>45</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="2:10">
       <c r="B58" s="1" t="s">
         <v>53</v>
       </c>
@@ -2839,23 +1937,17 @@
       <c r="G58" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H58" s="1" t="str">
-        <f>VLOOKUP($A58,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H58" t="s">
+        <v>38</v>
       </c>
       <c r="I58" s="1">
-        <f>VLOOKUP($A58,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J58" s="1">
-        <f>VLOOKUP($A58,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="1">
-        <v>45</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59" spans="2:10">
       <c r="B59" s="1" t="s">
         <v>54</v>
       </c>
@@ -2868,23 +1960,17 @@
       <c r="G59" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H59" s="1" t="str">
-        <f>VLOOKUP($A59,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H59" t="s">
+        <v>38</v>
       </c>
       <c r="I59" s="1">
-        <f>VLOOKUP($A59,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J59" s="1">
-        <f>VLOOKUP($A59,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
-      <c r="A60" s="1">
-        <v>54</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="60" spans="2:10">
       <c r="B60" s="1" t="s">
         <v>55</v>
       </c>
@@ -2897,23 +1983,17 @@
       <c r="G60" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H60" s="1" t="str">
-        <f>VLOOKUP($A60,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H60" t="s">
+        <v>38</v>
       </c>
       <c r="I60" s="1">
-        <f>VLOOKUP($A60,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J60" s="1">
-        <f>VLOOKUP($A60,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
-      <c r="A61" s="1">
-        <v>52</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="61" spans="2:10">
       <c r="B61" s="1" t="s">
         <v>56</v>
       </c>
@@ -2926,23 +2006,17 @@
       <c r="G61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H61" s="1" t="str">
-        <f>VLOOKUP($A61,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H61" t="s">
+        <v>38</v>
       </c>
       <c r="I61" s="1">
-        <f>VLOOKUP($A61,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J61" s="1">
-        <f>VLOOKUP($A61,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="1">
-        <v>55</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="2:10">
       <c r="B62" s="1" t="s">
         <v>57</v>
       </c>
@@ -2955,23 +2029,17 @@
       <c r="G62" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H62" s="1" t="str">
-        <f>VLOOKUP($A62,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H62" t="s">
+        <v>38</v>
       </c>
       <c r="I62" s="1">
-        <f>VLOOKUP($A62,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J62" s="1">
-        <f>VLOOKUP($A62,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="2:10">
       <c r="B63" s="1" t="s">
         <v>12</v>
       </c>
@@ -2984,23 +2052,17 @@
       <c r="G63" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H63" s="1" t="str">
-        <f>VLOOKUP($A63,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H63" t="s">
+        <v>38</v>
       </c>
       <c r="I63" s="1">
-        <f>VLOOKUP($A63,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J63" s="1">
-        <f>VLOOKUP($A63,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="2:10">
       <c r="B64" s="1" t="s">
         <v>13</v>
       </c>
@@ -3013,23 +2075,17 @@
       <c r="G64" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H64" s="1" t="str">
-        <f>VLOOKUP($A64,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H64" t="s">
+        <v>38</v>
       </c>
       <c r="I64" s="1">
-        <f>VLOOKUP($A64,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J64" s="1">
-        <f>VLOOKUP($A64,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10">
       <c r="B65" s="1" t="s">
         <v>58</v>
       </c>
@@ -3042,23 +2098,17 @@
       <c r="G65" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H65" s="1" t="str">
-        <f>VLOOKUP($A65,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H65" t="s">
+        <v>38</v>
       </c>
       <c r="I65" s="1">
-        <f>VLOOKUP($A65,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J65" s="1">
-        <f>VLOOKUP($A65,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10">
       <c r="B66" s="1" t="s">
         <v>59</v>
       </c>
@@ -3071,23 +2121,17 @@
       <c r="G66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H66" s="1" t="str">
-        <f>VLOOKUP($A66,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H66" t="s">
+        <v>38</v>
       </c>
       <c r="I66" s="1">
-        <f>VLOOKUP($A66,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J66" s="1">
-        <f>VLOOKUP($A66,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10">
       <c r="B67" s="1" t="s">
         <v>16</v>
       </c>
@@ -3100,23 +2144,17 @@
       <c r="G67" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H67" s="1" t="str">
-        <f>VLOOKUP($A67,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H67" t="s">
+        <v>38</v>
       </c>
       <c r="I67" s="1">
-        <f>VLOOKUP($A67,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J67" s="1">
-        <f>VLOOKUP($A67,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10">
       <c r="B68" s="1" t="s">
         <v>60</v>
       </c>
@@ -3129,23 +2167,17 @@
       <c r="G68" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H68" s="1" t="str">
-        <f>VLOOKUP($A68,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H68" t="s">
+        <v>38</v>
       </c>
       <c r="I68" s="1">
-        <f>VLOOKUP($A68,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J68" s="1">
-        <f>VLOOKUP($A68,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10">
       <c r="B69" s="1" t="s">
         <v>12</v>
       </c>
@@ -3158,23 +2190,17 @@
       <c r="G69" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H69" s="1" t="str">
-        <f>VLOOKUP($A69,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H69" t="s">
+        <v>38</v>
       </c>
       <c r="I69" s="1">
-        <f>VLOOKUP($A69,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J69" s="1">
-        <f>VLOOKUP($A69,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10">
       <c r="B70" s="1" t="s">
         <v>13</v>
       </c>
@@ -3187,23 +2213,17 @@
       <c r="G70" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H70" s="1" t="str">
-        <f>VLOOKUP($A70,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H70" t="s">
+        <v>38</v>
       </c>
       <c r="I70" s="1">
-        <f>VLOOKUP($A70,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J70" s="1">
-        <f>VLOOKUP($A70,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10">
       <c r="B71" s="1" t="s">
         <v>58</v>
       </c>
@@ -3216,23 +2236,17 @@
       <c r="G71" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H71" s="1" t="str">
-        <f>VLOOKUP($A71,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H71" t="s">
+        <v>38</v>
       </c>
       <c r="I71" s="1">
-        <f>VLOOKUP($A71,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J71" s="1">
-        <f>VLOOKUP($A71,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10">
       <c r="B72" s="1" t="s">
         <v>59</v>
       </c>
@@ -3245,23 +2259,17 @@
       <c r="G72" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H72" s="1" t="str">
-        <f>VLOOKUP($A72,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H72" t="s">
+        <v>38</v>
       </c>
       <c r="I72" s="1">
-        <f>VLOOKUP($A72,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J72" s="1">
-        <f>VLOOKUP($A72,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="2:10">
       <c r="B73" s="1" t="s">
         <v>16</v>
       </c>
@@ -3274,23 +2282,17 @@
       <c r="G73" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H73" s="1" t="str">
-        <f>VLOOKUP($A73,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H73" t="s">
+        <v>38</v>
       </c>
       <c r="I73" s="1">
-        <f>VLOOKUP($A73,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J73" s="1">
-        <f>VLOOKUP($A73,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" s="1">
-        <v>53</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10">
       <c r="B74" s="1" t="s">
         <v>60</v>
       </c>
@@ -3303,23 +2305,17 @@
       <c r="G74" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H74" s="1" t="str">
-        <f>VLOOKUP($A74,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H74" t="s">
+        <v>38</v>
       </c>
       <c r="I74" s="1">
-        <f>VLOOKUP($A74,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J74" s="1">
-        <f>VLOOKUP($A74,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" s="1">
-        <v>50</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10">
       <c r="B75" s="1" t="s">
         <v>18</v>
       </c>
@@ -3332,23 +2328,17 @@
       <c r="G75" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="H75" s="1" t="str">
-        <f>VLOOKUP($A75,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H75" t="s">
+        <v>38</v>
       </c>
       <c r="I75" s="1">
-        <f>VLOOKUP($A75,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J75" s="1">
-        <f>VLOOKUP($A75,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10">
       <c r="B76" s="1" t="s">
         <v>12</v>
       </c>
@@ -3361,23 +2351,17 @@
       <c r="G76" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H76" s="1" t="str">
-        <f>VLOOKUP($A76,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H76" t="s">
+        <v>38</v>
       </c>
       <c r="I76" s="1">
-        <f>VLOOKUP($A76,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J76" s="1">
-        <f>VLOOKUP($A76,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10">
       <c r="B77" s="1" t="s">
         <v>13</v>
       </c>
@@ -3390,23 +2374,17 @@
       <c r="G77" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H77" s="1" t="str">
-        <f>VLOOKUP($A77,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H77" t="s">
+        <v>38</v>
       </c>
       <c r="I77" s="1">
-        <f>VLOOKUP($A77,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J77" s="1">
-        <f>VLOOKUP($A77,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10">
       <c r="B78" s="1" t="s">
         <v>58</v>
       </c>
@@ -3419,23 +2397,17 @@
       <c r="G78" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H78" s="1" t="str">
-        <f>VLOOKUP($A78,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H78" t="s">
+        <v>38</v>
       </c>
       <c r="I78" s="1">
-        <f>VLOOKUP($A78,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J78" s="1">
-        <f>VLOOKUP($A78,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="79" spans="2:10">
       <c r="B79" s="1" t="s">
         <v>59</v>
       </c>
@@ -3448,23 +2420,17 @@
       <c r="G79" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H79" s="1" t="str">
-        <f>VLOOKUP($A79,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H79" t="s">
+        <v>38</v>
       </c>
       <c r="I79" s="1">
-        <f>VLOOKUP($A79,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J79" s="1">
-        <f>VLOOKUP($A79,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10">
       <c r="B80" s="1" t="s">
         <v>16</v>
       </c>
@@ -3477,23 +2443,17 @@
       <c r="G80" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H80" s="1" t="str">
-        <f>VLOOKUP($A80,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H80" t="s">
+        <v>38</v>
       </c>
       <c r="I80" s="1">
-        <f>VLOOKUP($A80,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J80" s="1">
-        <f>VLOOKUP($A80,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
-      <c r="A81" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="2:10">
       <c r="B81" s="1" t="s">
         <v>60</v>
       </c>
@@ -3506,23 +2466,17 @@
       <c r="G81" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H81" s="1" t="str">
-        <f>VLOOKUP($A81,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H81" t="s">
+        <v>38</v>
       </c>
       <c r="I81" s="1">
-        <f>VLOOKUP($A81,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J81" s="1">
-        <f>VLOOKUP($A81,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
-      <c r="A82" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10">
       <c r="B82" s="1" t="s">
         <v>12</v>
       </c>
@@ -3535,23 +2489,17 @@
       <c r="G82" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H82" s="1" t="str">
-        <f>VLOOKUP($A82,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H82" t="s">
+        <v>38</v>
       </c>
       <c r="I82" s="1">
-        <f>VLOOKUP($A82,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J82" s="1">
-        <f>VLOOKUP($A82,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="A83" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10">
       <c r="B83" s="1" t="s">
         <v>13</v>
       </c>
@@ -3564,23 +2512,17 @@
       <c r="G83" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H83" s="1" t="str">
-        <f>VLOOKUP($A83,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H83" t="s">
+        <v>38</v>
       </c>
       <c r="I83" s="1">
-        <f>VLOOKUP($A83,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J83" s="1">
-        <f>VLOOKUP($A83,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
-      <c r="A84" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="2:10">
       <c r="B84" s="1" t="s">
         <v>58</v>
       </c>
@@ -3593,23 +2535,17 @@
       <c r="G84" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H84" s="1" t="str">
-        <f>VLOOKUP($A84,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H84" t="s">
+        <v>38</v>
       </c>
       <c r="I84" s="1">
-        <f>VLOOKUP($A84,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J84" s="1">
-        <f>VLOOKUP($A84,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
-      <c r="A85" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="2:10">
       <c r="B85" s="1" t="s">
         <v>59</v>
       </c>
@@ -3622,23 +2558,17 @@
       <c r="G85" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H85" s="1" t="str">
-        <f>VLOOKUP($A85,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H85" t="s">
+        <v>38</v>
       </c>
       <c r="I85" s="1">
-        <f>VLOOKUP($A85,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J85" s="1">
-        <f>VLOOKUP($A85,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
-      <c r="A86" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="2:10">
       <c r="B86" s="1" t="s">
         <v>16</v>
       </c>
@@ -3651,23 +2581,17 @@
       <c r="G86" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H86" s="1" t="str">
-        <f>VLOOKUP($A86,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H86" t="s">
+        <v>38</v>
       </c>
       <c r="I86" s="1">
-        <f>VLOOKUP($A86,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J86" s="1">
-        <f>VLOOKUP($A86,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
-      <c r="A87" s="1">
-        <v>56</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="2:10">
       <c r="B87" s="1" t="s">
         <v>60</v>
       </c>
@@ -3680,20 +2604,17 @@
       <c r="G87" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H87" s="1" t="str">
-        <f>VLOOKUP($A87,[1]Sheet2!$A$2:$E$33,3,TRUE)</f>
-        <v>2017-2018</v>
+      <c r="H87" t="s">
+        <v>38</v>
       </c>
       <c r="I87" s="1">
-        <f>VLOOKUP($A87,[1]Sheet2!$A$2:$E$33,4,TRUE)</f>
         <v>2</v>
       </c>
       <c r="J87" s="1">
-        <f>VLOOKUP($A87,[1]Sheet2!$A$2:$E$33,5,TRUE)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="2:10">
       <c r="B88" t="s">
         <v>19</v>
       </c>
@@ -3718,7 +2639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="2:10">
       <c r="B89" t="s">
         <v>20</v>
       </c>
@@ -3743,7 +2664,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="2:10">
       <c r="B90" t="s">
         <v>21</v>
       </c>
@@ -3768,7 +2689,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="2:10">
       <c r="B91" t="s">
         <v>22</v>
       </c>
@@ -3793,7 +2714,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="2:10">
       <c r="B92" t="s">
         <v>23</v>
       </c>
@@ -3818,7 +2739,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="2:10">
       <c r="B93" t="s">
         <v>24</v>
       </c>
@@ -3843,7 +2764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="2:10">
       <c r="B94" t="s">
         <v>25</v>
       </c>
@@ -3868,7 +2789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="2:10">
       <c r="B95" t="s">
         <v>26</v>
       </c>
@@ -3893,7 +2814,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="2:10">
       <c r="B96" t="s">
         <v>27</v>
       </c>
@@ -6320,7 +5241,7 @@
     </row>
     <row r="187" spans="2:10">
       <c r="B187" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C187" t="s">
         <v>38</v>
@@ -6343,7 +5264,7 @@
     </row>
     <row r="188" spans="2:10">
       <c r="B188" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C188" t="s">
         <v>38</v>
@@ -6872,7 +5793,7 @@
     </row>
     <row r="211" spans="2:10">
       <c r="B211" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C211" t="s">
         <v>38</v>
@@ -6895,7 +5816,7 @@
     </row>
     <row r="212" spans="2:10">
       <c r="B212" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C212" t="s">
         <v>38</v>

</xml_diff>